<commit_message>
more study of veg comp
</commit_message>
<xml_diff>
--- a/output/ClusterAnalysisPerformance.xlsx
+++ b/output/ClusterAnalysisPerformance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace2\match_pedon_site\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65B5E5A-C3E0-4BA3-AF08-F9F90633BDED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB040AA3-5785-4450-BDEA-3633AAE12430}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5093B92A-DE42-4B02-9A90-566AE8194217}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{5093B92A-DE42-4B02-9A90-566AE8194217}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="performance" sheetId="1" r:id="rId1"/>
+    <sheet name="clustercomp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="76">
   <si>
     <t>klevel</t>
   </si>
@@ -121,6 +122,144 @@
   </si>
   <si>
     <t>mean 17-24</t>
+  </si>
+  <si>
+    <t>agnes.bray</t>
+  </si>
+  <si>
+    <t>agnes.jaccard</t>
+  </si>
+  <si>
+    <t>diana.jaccard</t>
+  </si>
+  <si>
+    <t>ward.bray</t>
+  </si>
+  <si>
+    <t>diana.bray</t>
+  </si>
+  <si>
+    <t>single.bray</t>
+  </si>
+  <si>
+    <t>complete.bray</t>
+  </si>
+  <si>
+    <t>agnes.simpson</t>
+  </si>
+  <si>
+    <t>ward.simpson</t>
+  </si>
+  <si>
+    <t>diana.simpson</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>province+ section</t>
+  </si>
+  <si>
+    <t>Cophenetic distances from province and section groupings</t>
+  </si>
+  <si>
+    <t>ward.jaccard</t>
+  </si>
+  <si>
+    <t>diana jaccard</t>
+  </si>
+  <si>
+    <t>diana bray</t>
+  </si>
+  <si>
+    <t>Fraxinus pennsylvanica/Phalaris arundinacea-Impatiens capensis</t>
+  </si>
+  <si>
+    <t>Wet Woodland</t>
+  </si>
+  <si>
+    <t>Acer saccharinum/Boehmeria cylindrica</t>
+  </si>
+  <si>
+    <t>Wet Deciduous Forest</t>
+  </si>
+  <si>
+    <t>Ulmus americana/Persicaria virginiana-Pilea pumila</t>
+  </si>
+  <si>
+    <t>Cornus racemosa/Carex stricta-Onoclea sensibilis</t>
+  </si>
+  <si>
+    <t>Wet Deciduous Shrubland</t>
+  </si>
+  <si>
+    <t>Wet Sparse</t>
+  </si>
+  <si>
+    <t>Juniperus virginiana/Carex lasiocarpa-Schoenoplectus pungens</t>
+  </si>
+  <si>
+    <t>Wet Shrubby Grassland</t>
+  </si>
+  <si>
+    <t>Cornus alba/Typha angustifolia-Eutrochium maculatum</t>
+  </si>
+  <si>
+    <t>Acer rubrum/Ilex verticillata</t>
+  </si>
+  <si>
+    <t>Salix nigra/Phalaris arundinacea-Boehmeria cylindrica</t>
+  </si>
+  <si>
+    <t>Fraxinus pennsylvanica/Impatiens capensis</t>
+  </si>
+  <si>
+    <t>Acer saccharinum/Cephalanthus occidentalis/Boehmeria cylindrica</t>
+  </si>
+  <si>
+    <t>Ulmus americana/Persicaria virginiana-Toxicodendron radicans</t>
+  </si>
+  <si>
+    <t>Typha angustifolia-Thelypteris palustris</t>
+  </si>
+  <si>
+    <t>Wet Grassland</t>
+  </si>
+  <si>
+    <t>Sambucus nigra/Symphyotrichum puniceum-Eutrochium maculatum</t>
+  </si>
+  <si>
+    <t>Acer saccharinum/Boehmeria cylindrica-Scutellaria lateriflora</t>
+  </si>
+  <si>
+    <t>Acer saccharinum/Cephalanthus occidentalis</t>
+  </si>
+  <si>
+    <t>Thelypteris palustris-Asclepias incarnata-Toxicodendron vernix</t>
+  </si>
+  <si>
+    <t>Salix discolor/Typha angustifolia-Lysimachia terrestris</t>
+  </si>
+  <si>
+    <t>cluster</t>
+  </si>
+  <si>
+    <t>sil_width</t>
+  </si>
+  <si>
+    <t>agnes</t>
+  </si>
+  <si>
+    <t>association</t>
+  </si>
+  <si>
+    <t>structure</t>
   </si>
 </sst>
 </file>
@@ -152,7 +291,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +316,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -230,11 +375,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCFD4D8"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCFD4D8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -270,6 +426,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,13 +755,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44202EFB-DF2D-460C-A98E-9C14A00CE468}">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="20" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="20" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1774,11 +1946,11 @@
         <v>0.32923905714285712</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" ref="D24:J24" si="0">AVERAGE(D4:D10)</f>
+        <f>AVERAGE(D4:D10)</f>
         <v>0.32542057142857139</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E24:J24" si="0">AVERAGE(E4:E10)</f>
         <v>0.30905231428571428</v>
       </c>
       <c r="F24" s="4">
@@ -2099,13 +2271,13 @@
         <v>5</v>
       </c>
       <c r="O32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>9</v>
@@ -2155,13 +2327,13 @@
         <v>8.0152780000000007E-2</v>
       </c>
       <c r="O33" s="4">
+        <v>8.492661E-2</v>
+      </c>
+      <c r="P33" s="4">
+        <v>5.8261069999999998E-2</v>
+      </c>
+      <c r="Q33" s="4">
         <v>7.6685680699999995E-2</v>
-      </c>
-      <c r="P33" s="4">
-        <v>8.492661E-2</v>
-      </c>
-      <c r="Q33" s="4">
-        <v>5.8261069999999998E-2</v>
       </c>
       <c r="R33" s="4">
         <v>6.5718550000000001E-2</v>
@@ -2211,13 +2383,13 @@
         <v>7.1905979999999994E-2</v>
       </c>
       <c r="O34" s="5">
+        <v>8.7314719999999998E-2</v>
+      </c>
+      <c r="P34" s="5">
+        <v>4.728885E-2</v>
+      </c>
+      <c r="Q34" s="5">
         <v>6.3453513500000003E-2</v>
-      </c>
-      <c r="P34" s="5">
-        <v>8.7314719999999998E-2</v>
-      </c>
-      <c r="Q34" s="5">
-        <v>4.728885E-2</v>
       </c>
       <c r="R34" s="5">
         <v>8.5091739999999999E-2</v>
@@ -2267,13 +2439,13 @@
         <v>6.7381620000000003E-2</v>
       </c>
       <c r="O35" s="4">
+        <v>9.6054719999999996E-2</v>
+      </c>
+      <c r="P35" s="4">
+        <v>7.0562689999999997E-2</v>
+      </c>
+      <c r="Q35" s="4">
         <v>2.0820033799999998E-2</v>
-      </c>
-      <c r="P35" s="4">
-        <v>9.6054719999999996E-2</v>
-      </c>
-      <c r="Q35" s="4">
-        <v>7.0562689999999997E-2</v>
       </c>
       <c r="R35" s="4">
         <v>0.10769165</v>
@@ -2323,13 +2495,13 @@
         <v>7.9542890000000005E-2</v>
       </c>
       <c r="O36" s="5">
+        <v>0.11482525</v>
+      </c>
+      <c r="P36" s="5">
+        <v>9.6525E-2</v>
+      </c>
+      <c r="Q36" s="5">
         <v>2.9392284000000001E-2</v>
-      </c>
-      <c r="P36" s="5">
-        <v>0.11482525</v>
-      </c>
-      <c r="Q36" s="5">
-        <v>9.6525E-2</v>
       </c>
       <c r="R36" s="5">
         <v>0.12958368000000001</v>
@@ -2379,13 +2551,13 @@
         <v>0.10377722</v>
       </c>
       <c r="O37" s="4">
+        <v>0.1276079</v>
+      </c>
+      <c r="P37" s="4">
+        <v>9.7203609999999996E-2</v>
+      </c>
+      <c r="Q37" s="4">
         <v>4.3522713900000003E-2</v>
-      </c>
-      <c r="P37" s="4">
-        <v>0.1276079</v>
-      </c>
-      <c r="Q37" s="4">
-        <v>9.7203609999999996E-2</v>
       </c>
       <c r="R37" s="4">
         <v>0.11684282999999999</v>
@@ -2435,13 +2607,13 @@
         <v>0.12271612</v>
       </c>
       <c r="O38" s="5">
+        <v>0.13226356</v>
+      </c>
+      <c r="P38" s="5">
+        <v>0.12304296000000001</v>
+      </c>
+      <c r="Q38" s="5">
         <v>3.9874407399999999E-2</v>
-      </c>
-      <c r="P38" s="5">
-        <v>0.13226356</v>
-      </c>
-      <c r="Q38" s="5">
-        <v>0.12304296000000001</v>
       </c>
       <c r="R38" s="5">
         <v>8.2205120000000007E-2</v>
@@ -2491,13 +2663,13 @@
         <v>0.13893907999999999</v>
       </c>
       <c r="O39" s="4">
+        <v>0.13815306999999999</v>
+      </c>
+      <c r="P39" s="4">
+        <v>0.13014969000000001</v>
+      </c>
+      <c r="Q39" s="4">
         <v>4.0912414199999997E-2</v>
-      </c>
-      <c r="P39" s="4">
-        <v>0.13815306999999999</v>
-      </c>
-      <c r="Q39" s="4">
-        <v>0.13014969000000001</v>
       </c>
       <c r="R39" s="4">
         <v>0.11028664000000001</v>
@@ -2547,13 +2719,13 @@
         <v>0.1302769</v>
       </c>
       <c r="O40" s="5">
+        <v>0.13348619</v>
+      </c>
+      <c r="P40" s="5">
+        <v>0.13703601000000001</v>
+      </c>
+      <c r="Q40" s="5">
         <v>3.9459518899999997E-2</v>
-      </c>
-      <c r="P40" s="5">
-        <v>0.13348619</v>
-      </c>
-      <c r="Q40" s="5">
-        <v>0.13703601000000001</v>
       </c>
       <c r="R40" s="5">
         <v>0.12470552999999999</v>
@@ -2603,13 +2775,13 @@
         <v>0.14546548000000001</v>
       </c>
       <c r="O41" s="4">
+        <v>0.14004204000000001</v>
+      </c>
+      <c r="P41" s="4">
+        <v>0.14568054</v>
+      </c>
+      <c r="Q41" s="4">
         <v>1.5938418999999999E-2</v>
-      </c>
-      <c r="P41" s="4">
-        <v>0.14004204000000001</v>
-      </c>
-      <c r="Q41" s="4">
-        <v>0.14568054</v>
       </c>
       <c r="R41" s="4">
         <v>0.13309001000000001</v>
@@ -2659,13 +2831,13 @@
         <v>0.14646192999999999</v>
       </c>
       <c r="O42" s="5">
+        <v>0.14332073000000001</v>
+      </c>
+      <c r="P42" s="5">
+        <v>0.14483401000000001</v>
+      </c>
+      <c r="Q42" s="5">
         <v>1.00483608E-2</v>
-      </c>
-      <c r="P42" s="5">
-        <v>0.14332073000000001</v>
-      </c>
-      <c r="Q42" s="5">
-        <v>0.14483401000000001</v>
       </c>
       <c r="R42" s="5">
         <v>0.11040423000000001</v>
@@ -2715,13 +2887,13 @@
         <v>0.14989398000000001</v>
       </c>
       <c r="O43" s="4">
+        <v>0.15118059</v>
+      </c>
+      <c r="P43" s="4">
+        <v>0.15000632</v>
+      </c>
+      <c r="Q43" s="4">
         <v>6.2689060000000005E-4</v>
-      </c>
-      <c r="P43" s="4">
-        <v>0.15118059</v>
-      </c>
-      <c r="Q43" s="4">
-        <v>0.15000632</v>
       </c>
       <c r="R43" s="4">
         <v>0.12501662999999999</v>
@@ -2771,13 +2943,13 @@
         <v>0.14966668</v>
       </c>
       <c r="O44" s="5">
+        <v>0.15066251</v>
+      </c>
+      <c r="P44" s="5">
+        <v>0.15355785999999999</v>
+      </c>
+      <c r="Q44" s="5">
         <v>-1.0820869300000001E-2</v>
-      </c>
-      <c r="P44" s="5">
-        <v>0.15066251</v>
-      </c>
-      <c r="Q44" s="5">
-        <v>0.15355785999999999</v>
       </c>
       <c r="R44" s="5">
         <v>0.12985060000000001</v>
@@ -2827,13 +2999,13 @@
         <v>0.1550165</v>
       </c>
       <c r="O45" s="4">
+        <v>0.15186833999999999</v>
+      </c>
+      <c r="P45" s="4">
+        <v>0.16019968000000001</v>
+      </c>
+      <c r="Q45" s="4">
         <v>1.4203967099999999E-2</v>
-      </c>
-      <c r="P45" s="4">
-        <v>0.15186833999999999</v>
-      </c>
-      <c r="Q45" s="4">
-        <v>0.16019968000000001</v>
       </c>
       <c r="R45" s="4">
         <v>0.11302357</v>
@@ -2883,13 +3055,13 @@
         <v>0.16331156999999999</v>
       </c>
       <c r="O46" s="5">
+        <v>0.15604698</v>
+      </c>
+      <c r="P46" s="5">
+        <v>0.15539304000000001</v>
+      </c>
+      <c r="Q46" s="5">
         <v>-3.2236795999999999E-3</v>
-      </c>
-      <c r="P46" s="5">
-        <v>0.15604698</v>
-      </c>
-      <c r="Q46" s="5">
-        <v>0.15539304000000001</v>
       </c>
       <c r="R46" s="5">
         <v>0.13038063</v>
@@ -2939,13 +3111,13 @@
         <v>0.16713063</v>
       </c>
       <c r="O47" s="4">
+        <v>0.15016113</v>
+      </c>
+      <c r="P47" s="4">
+        <v>0.14779867999999999</v>
+      </c>
+      <c r="Q47" s="4">
         <v>2.0771132999999999E-3</v>
-      </c>
-      <c r="P47" s="4">
-        <v>0.15016113</v>
-      </c>
-      <c r="Q47" s="4">
-        <v>0.14779867999999999</v>
       </c>
       <c r="R47" s="4">
         <v>0.12265613</v>
@@ -2995,13 +3167,13 @@
         <v>0.16052453999999999</v>
       </c>
       <c r="O48" s="5">
+        <v>0.15397354999999999</v>
+      </c>
+      <c r="P48" s="5">
+        <v>0.14468424999999999</v>
+      </c>
+      <c r="Q48" s="5">
         <v>-2.2882590500000001E-2</v>
-      </c>
-      <c r="P48" s="5">
-        <v>0.15397354999999999</v>
-      </c>
-      <c r="Q48" s="5">
-        <v>0.14468424999999999</v>
       </c>
       <c r="R48" s="5">
         <v>0.12495071000000001</v>
@@ -3051,13 +3223,13 @@
         <v>0.14771449</v>
       </c>
       <c r="O49" s="4">
+        <v>0.15663328000000001</v>
+      </c>
+      <c r="P49" s="4">
+        <v>0.13230916000000001</v>
+      </c>
+      <c r="Q49" s="4">
         <v>-3.2455868200000001E-2</v>
-      </c>
-      <c r="P49" s="4">
-        <v>0.15663328000000001</v>
-      </c>
-      <c r="Q49" s="4">
-        <v>0.13230916000000001</v>
       </c>
       <c r="R49" s="4">
         <v>0.12331004</v>
@@ -3107,13 +3279,13 @@
         <v>0.14452778999999999</v>
       </c>
       <c r="O50" s="5">
+        <v>0.15491596999999999</v>
+      </c>
+      <c r="P50" s="5">
+        <v>0.13783065</v>
+      </c>
+      <c r="Q50" s="5">
         <v>-3.6365560800000002E-2</v>
-      </c>
-      <c r="P50" s="5">
-        <v>0.15491596999999999</v>
-      </c>
-      <c r="Q50" s="5">
-        <v>0.13783065</v>
       </c>
       <c r="R50" s="5">
         <v>0.11145803999999999</v>
@@ -3163,13 +3335,13 @@
         <v>0.14501066000000001</v>
       </c>
       <c r="O51" s="4">
+        <v>0.14672732999999999</v>
+      </c>
+      <c r="P51" s="4">
+        <v>0.12655443</v>
+      </c>
+      <c r="Q51" s="4">
         <v>-3.58992162E-2</v>
-      </c>
-      <c r="P51" s="4">
-        <v>0.14672732999999999</v>
-      </c>
-      <c r="Q51" s="4">
-        <v>0.12655443</v>
       </c>
       <c r="R51" s="4">
         <v>9.7814799999999993E-2</v>
@@ -3229,16 +3401,16 @@
         <v>9.4916527142857143E-2</v>
       </c>
       <c r="O53" s="4">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(O33:O39)</f>
+        <v>0.11159226142857144</v>
+      </c>
+      <c r="P53" s="4">
+        <f>AVERAGE(P33:P39)</f>
+        <v>8.9004838571428574E-2</v>
+      </c>
+      <c r="Q53" s="4">
+        <f>AVERAGE(Q33:Q39)</f>
         <v>4.4951578214285713E-2</v>
-      </c>
-      <c r="P53" s="4">
-        <f t="shared" si="7"/>
-        <v>0.11159226142857144</v>
-      </c>
-      <c r="Q53" s="4">
-        <f t="shared" si="7"/>
-        <v>8.9004838571428574E-2</v>
       </c>
       <c r="R53" s="4">
         <f t="shared" si="7"/>
@@ -3301,16 +3473,16 @@
         <v>0.15090295874999998</v>
       </c>
       <c r="O54" s="5">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(O40:O47)</f>
+        <v>0.14709606375000001</v>
+      </c>
+      <c r="P54" s="5">
+        <f>AVERAGE(P40:P47)</f>
+        <v>0.14931326750000001</v>
+      </c>
+      <c r="Q54" s="5">
+        <f>AVERAGE(Q40:Q47)</f>
         <v>8.5387151000000001E-3</v>
-      </c>
-      <c r="P54" s="5">
-        <f t="shared" si="9"/>
-        <v>0.14709606375000001</v>
-      </c>
-      <c r="Q54" s="5">
-        <f t="shared" si="9"/>
-        <v>0.14931326750000001</v>
       </c>
       <c r="R54" s="5">
         <f t="shared" si="9"/>
@@ -3373,16 +3545,16 @@
         <v>3</v>
       </c>
       <c r="O56" s="9">
-        <f t="shared" si="11"/>
+        <f>RANK(O53,($M53:$T53))</f>
+        <v>1</v>
+      </c>
+      <c r="P56" s="9">
+        <f>RANK(P53,($M53:$T53))</f>
+        <v>5</v>
+      </c>
+      <c r="Q56" s="9">
+        <f>RANK(Q53,($M53:$T53))</f>
         <v>8</v>
-      </c>
-      <c r="P56" s="9">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="Q56" s="9">
-        <f t="shared" si="11"/>
-        <v>5</v>
       </c>
       <c r="R56" s="9">
         <f t="shared" si="11"/>
@@ -3445,16 +3617,16 @@
         <v>1</v>
       </c>
       <c r="O57" s="9">
-        <f t="shared" si="11"/>
+        <f>RANK(O54,($M54:$T54))</f>
+        <v>4</v>
+      </c>
+      <c r="P57" s="9">
+        <f>RANK(P54,($M54:$T54))</f>
+        <v>3</v>
+      </c>
+      <c r="Q57" s="9">
+        <f>RANK(Q54,($M54:$T54))</f>
         <v>8</v>
-      </c>
-      <c r="P57" s="9">
-        <f t="shared" si="11"/>
-        <v>4</v>
-      </c>
-      <c r="Q57" s="9">
-        <f t="shared" si="11"/>
-        <v>3</v>
       </c>
       <c r="R57" s="9">
         <f t="shared" si="11"/>
@@ -3979,15 +4151,15 @@
         <v>0.23089412199999998</v>
       </c>
       <c r="P76" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(E82,E53,Q53,O24,E24)</f>
         <v>0.19587889684285714</v>
       </c>
       <c r="Q76" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(F82,F53,O53,P24,F24)</f>
         <v>0.22260635314285712</v>
       </c>
       <c r="R76" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(G82,G53,P53,Q24,G24)</f>
         <v>0.21201107857142856</v>
       </c>
       <c r="S76" s="14">
@@ -4043,15 +4215,15 @@
         <v>0.20638305125</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(E83,E54,Q54,O25,E25)</f>
         <v>0.11530282442000002</v>
       </c>
       <c r="Q77" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(F83,F54,O54,P25,F25)</f>
         <v>0.20127402974999997</v>
       </c>
       <c r="R77" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(G83,G54,P54,Q25,G25)</f>
         <v>0.18952693849999999</v>
       </c>
       <c r="S77" s="14">
@@ -4224,7 +4396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
@@ -4234,7 +4406,7 @@
       <c r="I81" s="6"/>
       <c r="J81" s="6"/>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>1</v>
       </c>
@@ -4271,7 +4443,7 @@
         <v>0.23821479285714289</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>2</v>
       </c>
@@ -4308,7 +4480,7 @@
         <v>0.1465071325</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B85" s="9" t="s">
         <v>3</v>
       </c>
@@ -4345,7 +4517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
         <v>3</v>
       </c>
@@ -4382,12 +4554,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B89" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="90" spans="2:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="L89" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" ht="21" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>0</v>
       </c>
@@ -4404,19 +4579,34 @@
         <v>7</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H90" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I90" s="1" t="s">
+      <c r="J90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J90" s="1" t="s">
+      <c r="K90" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
         <v>2</v>
       </c>
@@ -4436,16 +4626,31 @@
         <v>0.30201670000000003</v>
       </c>
       <c r="H91" s="4">
+        <v>0.30168279999999997</v>
+      </c>
+      <c r="I91" s="4">
         <v>0.30238700000000002</v>
       </c>
-      <c r="I91" s="4">
+      <c r="J91" s="4">
         <v>0.17573560199999999</v>
       </c>
-      <c r="J91" s="4">
+      <c r="K91" s="4">
         <v>0.29048429999999997</v>
       </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M91" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N91" s="14">
+        <v>0.18403120000000001</v>
+      </c>
+      <c r="O91" s="14">
+        <v>0.1478797</v>
+      </c>
+      <c r="P91" s="14">
+        <v>0.20247879999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
         <v>3</v>
       </c>
@@ -4465,16 +4670,31 @@
         <v>0.26660610000000001</v>
       </c>
       <c r="H92" s="4">
+        <v>0.2637024</v>
+      </c>
+      <c r="I92" s="4">
         <v>0.24926409999999999</v>
       </c>
-      <c r="I92" s="4">
+      <c r="J92" s="4">
         <v>6.6698909999999998E-3</v>
       </c>
-      <c r="J92" s="4">
+      <c r="K92" s="4">
         <v>0.27802690000000002</v>
       </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M92" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N92" s="14">
+        <v>0.25853409999999999</v>
+      </c>
+      <c r="O92" s="14">
+        <v>0.12990209999999999</v>
+      </c>
+      <c r="P92" s="14">
+        <v>0.26078639999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
         <v>4</v>
       </c>
@@ -4494,16 +4714,31 @@
         <v>0.23640530000000001</v>
       </c>
       <c r="H93" s="4">
+        <v>0.22133420000000001</v>
+      </c>
+      <c r="I93" s="4">
         <v>0.2381182</v>
       </c>
-      <c r="I93" s="4">
+      <c r="J93" s="4">
         <v>-1.2969458E-2</v>
       </c>
-      <c r="J93" s="4">
+      <c r="K93" s="4">
         <v>0.22374849999999999</v>
       </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M93" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N93" s="14">
+        <v>0.33100950000000001</v>
+      </c>
+      <c r="O93" s="14">
+        <v>0.14888699999999999</v>
+      </c>
+      <c r="P93" s="14">
+        <v>0.32859450000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
         <v>5</v>
       </c>
@@ -4523,16 +4758,31 @@
         <v>0.216947</v>
       </c>
       <c r="H94" s="4">
+        <v>0.21555949999999999</v>
+      </c>
+      <c r="I94" s="4">
         <v>0.21806139999999999</v>
       </c>
-      <c r="I94" s="4">
+      <c r="J94" s="4">
         <v>-3.1514190999999997E-2</v>
       </c>
-      <c r="J94" s="4">
+      <c r="K94" s="4">
         <v>0.20963580000000001</v>
       </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M94" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N94" s="14">
+        <v>0.33348349999999999</v>
+      </c>
+      <c r="O94" s="14">
+        <v>0.1571698</v>
+      </c>
+      <c r="P94" s="14">
+        <v>0.33322990000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
         <v>6</v>
       </c>
@@ -4552,16 +4802,31 @@
         <v>0.23262869999999999</v>
       </c>
       <c r="H95" s="4">
+        <v>0.23182249999999999</v>
+      </c>
+      <c r="I95" s="4">
         <v>0.229931</v>
       </c>
-      <c r="I95" s="4">
+      <c r="J95" s="4">
         <v>-7.3522920000000005E-2</v>
       </c>
-      <c r="J95" s="4">
+      <c r="K95" s="4">
         <v>0.23089409999999999</v>
       </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N95" s="14">
+        <v>0.34730729999999999</v>
+      </c>
+      <c r="O95" s="14">
+        <v>0.21638199999999999</v>
+      </c>
+      <c r="P95" s="14">
+        <v>0.3630623</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
         <v>7</v>
       </c>
@@ -4581,16 +4846,31 @@
         <v>0.24773200000000001</v>
       </c>
       <c r="H96" s="4">
+        <v>0.22754840000000001</v>
+      </c>
+      <c r="I96" s="4">
         <v>0.23519909999999999</v>
       </c>
-      <c r="I96" s="4">
+      <c r="J96" s="4">
         <v>-8.0423701E-2</v>
       </c>
-      <c r="J96" s="4">
+      <c r="K96" s="4">
         <v>0.21888850000000001</v>
       </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M96" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N96" s="14">
+        <v>0.36988409999999999</v>
+      </c>
+      <c r="O96" s="14">
+        <v>0.18537729999999999</v>
+      </c>
+      <c r="P96" s="14">
+        <v>0.37296259999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
         <v>8</v>
       </c>
@@ -4610,16 +4890,31 @@
         <v>0.2456277</v>
       </c>
       <c r="H97" s="4">
+        <v>0.2441604</v>
+      </c>
+      <c r="I97" s="4">
         <v>0.25540059999999998</v>
       </c>
-      <c r="I97" s="4">
+      <c r="J97" s="4">
         <v>-8.8707907000000003E-2</v>
       </c>
-      <c r="J97" s="4">
+      <c r="K97" s="4">
         <v>0.2230104</v>
       </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M97" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N97" s="14">
+        <v>0.37049569999999998</v>
+      </c>
+      <c r="O97" s="14">
+        <v>0.24991650000000001</v>
+      </c>
+      <c r="P97" s="14">
+        <v>0.39310499999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
         <v>9</v>
       </c>
@@ -4639,16 +4934,31 @@
         <v>0.2385824</v>
       </c>
       <c r="H98" s="4">
+        <v>0.23755019999999999</v>
+      </c>
+      <c r="I98" s="4">
         <v>0.2216764</v>
       </c>
-      <c r="I98" s="4">
+      <c r="J98" s="4">
         <v>-0.142604484</v>
       </c>
-      <c r="J98" s="4">
+      <c r="K98" s="4">
         <v>0.22951840000000001</v>
       </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M98" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N98" s="14">
+        <v>0.40036339999999998</v>
+      </c>
+      <c r="O98" s="14">
+        <v>0.24887229999999999</v>
+      </c>
+      <c r="P98" s="14">
+        <v>0.41835349999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
         <v>10</v>
       </c>
@@ -4668,16 +4978,31 @@
         <v>0.24888979999999999</v>
       </c>
       <c r="H99" s="4">
+        <v>0.2231853</v>
+      </c>
+      <c r="I99" s="4">
         <v>0.2133496</v>
       </c>
-      <c r="I99" s="4">
+      <c r="J99" s="4">
         <v>-0.14366968199999999</v>
       </c>
-      <c r="J99" s="4">
+      <c r="K99" s="4">
         <v>0.22563250000000001</v>
       </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M99" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N99" s="14">
+        <v>0.41729270000000002</v>
+      </c>
+      <c r="O99" s="14">
+        <v>0.27189570000000002</v>
+      </c>
+      <c r="P99" s="14">
+        <v>0.43984329999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
         <v>11</v>
       </c>
@@ -4697,16 +5022,31 @@
         <v>0.2381086</v>
       </c>
       <c r="H100" s="4">
+        <v>0.2216784</v>
+      </c>
+      <c r="I100" s="4">
         <v>0.22412750000000001</v>
       </c>
-      <c r="I100" s="4">
+      <c r="J100" s="4">
         <v>-0.156536589</v>
       </c>
-      <c r="J100" s="4">
+      <c r="K100" s="4">
         <v>0.21570249999999999</v>
       </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M100" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N100" s="14">
+        <v>0.44091970000000003</v>
+      </c>
+      <c r="O100" s="14">
+        <v>0.29160079999999999</v>
+      </c>
+      <c r="P100" s="14">
+        <v>0.46605740000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
         <v>12</v>
       </c>
@@ -4726,16 +5066,31 @@
         <v>0.24052080000000001</v>
       </c>
       <c r="H101" s="4">
+        <v>0.23706630000000001</v>
+      </c>
+      <c r="I101" s="4">
         <v>0.24082909999999999</v>
       </c>
-      <c r="I101" s="4">
+      <c r="J101" s="4">
         <v>-0.16273099999999999</v>
       </c>
-      <c r="J101" s="4">
+      <c r="K101" s="4">
         <v>0.2264468</v>
       </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M101" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N101" s="14">
+        <v>0.43080220000000002</v>
+      </c>
+      <c r="O101" s="14">
+        <v>0.33461249999999998</v>
+      </c>
+      <c r="P101" s="14">
+        <v>0.470472</v>
+      </c>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B102" s="2">
         <v>13</v>
       </c>
@@ -4755,16 +5110,19 @@
         <v>0.2415117</v>
       </c>
       <c r="H102" s="4">
+        <v>0.23682310000000001</v>
+      </c>
+      <c r="I102" s="4">
         <v>0.1864748</v>
       </c>
-      <c r="I102" s="4">
+      <c r="J102" s="4">
         <v>-0.19005804700000001</v>
       </c>
-      <c r="J102" s="4">
+      <c r="K102" s="4">
         <v>0.218888</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B103" s="2">
         <v>14</v>
       </c>
@@ -4784,16 +5142,19 @@
         <v>0.24603369999999999</v>
       </c>
       <c r="H103" s="4">
+        <v>0.24337539999999999</v>
+      </c>
+      <c r="I103" s="4">
         <v>0.20202829999999999</v>
       </c>
-      <c r="I103" s="4">
+      <c r="J103" s="4">
         <v>-0.191709413</v>
       </c>
-      <c r="J103" s="4">
+      <c r="K103" s="4">
         <v>0.21635879999999999</v>
       </c>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B104" s="2">
         <v>15</v>
       </c>
@@ -4813,16 +5174,19 @@
         <v>0.2448207</v>
       </c>
       <c r="H104" s="4">
+        <v>0.24295910000000001</v>
+      </c>
+      <c r="I104" s="4">
         <v>0.25093500000000002</v>
       </c>
-      <c r="I104" s="4">
+      <c r="J104" s="4">
         <v>-0.19013954</v>
       </c>
-      <c r="J104" s="4">
+      <c r="K104" s="4">
         <v>0.20541870000000001</v>
       </c>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B105" s="2">
         <v>16</v>
       </c>
@@ -4842,16 +5206,19 @@
         <v>0.243531</v>
       </c>
       <c r="H105" s="4">
+        <v>0.24242900000000001</v>
+      </c>
+      <c r="I105" s="4">
         <v>0.2406645</v>
       </c>
-      <c r="I105" s="4">
+      <c r="J105" s="4">
         <v>-0.19193113000000001</v>
       </c>
-      <c r="J105" s="4">
+      <c r="K105" s="4">
         <v>0.2042012</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" s="2">
         <v>17</v>
       </c>
@@ -4871,16 +5238,19 @@
         <v>0.22930449999999999</v>
       </c>
       <c r="H106" s="4">
+        <v>0.23614470000000001</v>
+      </c>
+      <c r="I106" s="4">
         <v>0.21837119999999999</v>
       </c>
-      <c r="I106" s="4">
+      <c r="J106" s="4">
         <v>-0.19302629700000001</v>
       </c>
-      <c r="J106" s="4">
+      <c r="K106" s="4">
         <v>0.20449709999999999</v>
       </c>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B107" s="2">
         <v>18</v>
       </c>
@@ -4900,16 +5270,19 @@
         <v>0.22845170000000001</v>
       </c>
       <c r="H107" s="4">
+        <v>0.23505210000000001</v>
+      </c>
+      <c r="I107" s="4">
         <v>0.19531609999999999</v>
       </c>
-      <c r="I107" s="4">
+      <c r="J107" s="4">
         <v>-0.19728345</v>
       </c>
-      <c r="J107" s="4">
+      <c r="K107" s="4">
         <v>0.2075167</v>
       </c>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B108" s="2">
         <v>19</v>
       </c>
@@ -4929,16 +5302,19 @@
         <v>0.20660800000000001</v>
       </c>
       <c r="H108" s="4">
+        <v>0.236461</v>
+      </c>
+      <c r="I108" s="4">
         <v>0.20879719999999999</v>
       </c>
-      <c r="I108" s="4">
+      <c r="J108" s="4">
         <v>-0.20773366300000001</v>
       </c>
-      <c r="J108" s="4">
+      <c r="K108" s="4">
         <v>0.20595050000000001</v>
       </c>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B109" s="2">
         <v>20</v>
       </c>
@@ -4958,16 +5334,19 @@
         <v>0.20769599999999999</v>
       </c>
       <c r="H109" s="4">
+        <v>0.232402</v>
+      </c>
+      <c r="I109" s="4">
         <v>0.1831054</v>
       </c>
-      <c r="I109" s="4">
+      <c r="J109" s="4">
         <v>-0.20740045500000001</v>
       </c>
-      <c r="J109" s="4">
+      <c r="K109" s="4">
         <v>0.20764369999999999</v>
       </c>
     </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B110" s="2">
         <v>21</v>
       </c>
@@ -4987,16 +5366,19 @@
         <v>0.21653749999999999</v>
       </c>
       <c r="H110" s="4">
+        <v>0.2140232</v>
+      </c>
+      <c r="I110" s="4">
         <v>0.19553889999999999</v>
       </c>
-      <c r="I110" s="4">
+      <c r="J110" s="4">
         <v>-0.21626730399999999</v>
       </c>
-      <c r="J110" s="4">
+      <c r="K110" s="4">
         <v>0.20568220000000001</v>
       </c>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B111" s="2">
         <v>22</v>
       </c>
@@ -5016,16 +5398,19 @@
         <v>0.20359099999999999</v>
       </c>
       <c r="H111" s="4">
+        <v>0.21331839999999999</v>
+      </c>
+      <c r="I111" s="4">
         <v>0.1920038</v>
       </c>
-      <c r="I111" s="4">
+      <c r="J111" s="4">
         <v>-0.209812794</v>
       </c>
-      <c r="J111" s="4">
+      <c r="K111" s="4">
         <v>0.21178820000000001</v>
       </c>
     </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B112" s="2">
         <v>23</v>
       </c>
@@ -5045,16 +5430,19 @@
         <v>0.20003199999999999</v>
       </c>
       <c r="H112" s="4">
+        <v>0.220217</v>
+      </c>
+      <c r="I112" s="4">
         <v>0.2010372</v>
       </c>
-      <c r="I112" s="4">
+      <c r="J112" s="4">
         <v>-0.21431972899999999</v>
       </c>
-      <c r="J112" s="4">
+      <c r="K112" s="4">
         <v>0.2118623</v>
       </c>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B113" s="2">
         <v>24</v>
       </c>
@@ -5074,16 +5462,19 @@
         <v>0.19672680000000001</v>
       </c>
       <c r="H113" s="4">
+        <v>0.21621960000000001</v>
+      </c>
+      <c r="I113" s="4">
         <v>0.1947468</v>
       </c>
-      <c r="I113" s="4">
+      <c r="J113" s="4">
         <v>-0.21395455499999999</v>
       </c>
-      <c r="J113" s="4">
+      <c r="K113" s="4">
         <v>0.19668060000000001</v>
       </c>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
@@ -5092,82 +5483,91 @@
       <c r="H114" s="6"/>
       <c r="I114" s="6"/>
       <c r="J114" s="6"/>
-    </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K114" s="6"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C115" s="4">
-        <f>AVERAGE(C95:C101)</f>
-        <v>0.2510903285714286</v>
+        <f>AVERAGE(C91:C97)</f>
+        <v>0.25042015714285715</v>
       </c>
       <c r="D115" s="4">
-        <f t="shared" ref="D115:J115" si="17">AVERAGE(D95:D101)</f>
-        <v>0.24775229999999998</v>
+        <f t="shared" ref="D115:K115" si="17">AVERAGE(D91:D97)</f>
+        <v>0.24870312857142857</v>
       </c>
       <c r="E115" s="4">
         <f t="shared" si="17"/>
-        <v>0.22158087142857141</v>
+        <v>0.24132124285714288</v>
       </c>
       <c r="F115" s="4">
         <f t="shared" si="17"/>
-        <v>0.22919742857142858</v>
+        <v>0.24276407142857143</v>
       </c>
       <c r="G115" s="4">
         <f t="shared" si="17"/>
-        <v>0.24172714285714283</v>
+        <v>0.24970907142857146</v>
       </c>
       <c r="H115" s="4">
-        <f t="shared" si="17"/>
-        <v>0.23150190000000001</v>
+        <f>AVERAGE(H91:H97)</f>
+        <v>0.24368717142857141</v>
       </c>
       <c r="I115" s="4">
         <f t="shared" si="17"/>
-        <v>-0.12117089757142856</v>
+        <v>0.24690877142857143</v>
       </c>
       <c r="J115" s="4">
         <f t="shared" si="17"/>
-        <v>0.22429902857142855</v>
-      </c>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+        <v>-1.4961812E-2</v>
+      </c>
+      <c r="K115" s="4">
+        <f t="shared" si="17"/>
+        <v>0.23924121428571429</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C116" s="5">
-        <f>AVERAGE(C102:C109)</f>
-        <v>0.22792448749999999</v>
+        <f>AVERAGE(C98:C105)</f>
+        <v>0.24322308749999999</v>
       </c>
       <c r="D116" s="5">
-        <f t="shared" ref="D116:J117" si="18">AVERAGE(D102:D109)</f>
-        <v>0.22897215000000001</v>
+        <f t="shared" ref="D116:K116" si="18">AVERAGE(D98:D105)</f>
+        <v>0.2396903625</v>
       </c>
       <c r="E116" s="5">
         <f t="shared" si="18"/>
-        <v>0.22097011249999998</v>
+        <v>0.22448148749999999</v>
       </c>
       <c r="F116" s="5">
         <f t="shared" si="18"/>
-        <v>0.21621612500000001</v>
+        <v>0.220131725</v>
       </c>
       <c r="G116" s="5">
         <f t="shared" si="18"/>
-        <v>0.2309946625</v>
+        <v>0.24274983749999998</v>
       </c>
       <c r="H116" s="5">
-        <f t="shared" si="18"/>
-        <v>0.21071156250000003</v>
+        <f>AVERAGE(H98:H105)</f>
+        <v>0.23563334999999999</v>
       </c>
       <c r="I116" s="5">
         <f t="shared" si="18"/>
-        <v>-0.19616024937499998</v>
+        <v>0.22251065</v>
       </c>
       <c r="J116" s="5">
         <f t="shared" si="18"/>
-        <v>0.2088093375</v>
-      </c>
-    </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+        <v>-0.17117248562499998</v>
+      </c>
+      <c r="K116" s="5">
+        <f t="shared" si="18"/>
+        <v>0.21777086250000002</v>
+      </c>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>29</v>
       </c>
@@ -5176,7 +5576,7 @@
         <v>0.22956126250000003</v>
       </c>
       <c r="D117" s="5">
-        <f t="shared" ref="D117:J117" si="19">AVERAGE(D106:D113)</f>
+        <f t="shared" ref="D117:K117" si="19">AVERAGE(D106:D113)</f>
         <v>0.23393267500000001</v>
       </c>
       <c r="E117" s="5">
@@ -5192,132 +5592,151 @@
         <v>0.21111843750000001</v>
       </c>
       <c r="H117" s="5">
+        <f t="shared" ref="H117" si="20">AVERAGE(H106:H113)</f>
+        <v>0.22547974999999998</v>
+      </c>
+      <c r="I117" s="5">
         <f t="shared" si="19"/>
         <v>0.19861457500000002</v>
       </c>
-      <c r="I117" s="5">
+      <c r="J117" s="5">
         <f t="shared" si="19"/>
         <v>-0.20747478087500001</v>
       </c>
-      <c r="J117" s="5">
+      <c r="K117" s="5">
         <f t="shared" si="19"/>
         <v>0.20645266249999999</v>
       </c>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B119" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C119" s="9">
-        <f>RANK(C115,($C115:$J115))</f>
+        <f t="shared" ref="C119:K119" si="21">RANK(C115,($C115:$K115))</f>
         <v>1</v>
       </c>
       <c r="D119" s="9">
-        <f>RANK(D115,($C115:$J115))</f>
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="E119" s="9">
+        <f t="shared" si="21"/>
+        <v>7</v>
+      </c>
+      <c r="F119" s="9">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+      <c r="G119" s="9">
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="E119" s="9">
-        <f>RANK(E115,($C115:$J115))</f>
-        <v>7</v>
-      </c>
-      <c r="F119" s="9">
-        <f>RANK(F115,($C115:$J115))</f>
+      <c r="H119" s="9">
+        <f t="shared" si="21"/>
         <v>5</v>
       </c>
-      <c r="G119" s="9">
-        <f>RANK(G115,($C115:$J115))</f>
-        <v>3</v>
-      </c>
-      <c r="H119" s="9">
-        <f>RANK(H115,($C115:$J115))</f>
+      <c r="I119" s="9">
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
-      <c r="I119" s="9">
-        <f>RANK(I115,($C115:$J115))</f>
+      <c r="J119" s="9">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="K119" s="9">
+        <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="J119" s="9">
-        <f>RANK(J115,($C115:$J115))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C120" s="9">
-        <f>RANK(C116,($C116:$J116))</f>
+        <f t="shared" ref="C120:K120" si="22">RANK(C116,($C116:$K116))</f>
+        <v>1</v>
+      </c>
+      <c r="D120" s="9">
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
-      <c r="D120" s="9">
-        <f>RANK(D116,($C116:$J116))</f>
+      <c r="E120" s="9">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="F120" s="9">
+        <f t="shared" si="22"/>
+        <v>7</v>
+      </c>
+      <c r="G120" s="9">
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="E120" s="9">
-        <f>RANK(E116,($C116:$J116))</f>
+      <c r="H120" s="9">
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
-      <c r="F120" s="9">
-        <f>RANK(F116,($C116:$J116))</f>
-        <v>5</v>
-      </c>
-      <c r="G120" s="9">
-        <f>RANK(G116,($C116:$J116))</f>
-        <v>1</v>
-      </c>
-      <c r="H120" s="9">
-        <f>RANK(H116,($C116:$J116))</f>
+      <c r="I120" s="9">
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
-      <c r="I120" s="9">
-        <f>RANK(I116,($C116:$J116))</f>
+      <c r="J120" s="9">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="K120" s="9">
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
-      <c r="J120" s="9">
-        <f>RANK(J116,($C116:$J116))</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C121" s="9">
-        <f>RANK(C117,($C117:$J117))</f>
+        <f t="shared" ref="C121:K121" si="23">RANK(C117,($C117:$K117))</f>
         <v>2</v>
       </c>
       <c r="D121" s="9">
-        <f>RANK(D117,($C117:$J117))</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="E121" s="9">
-        <f>RANK(E117,($C117:$J117))</f>
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="F121" s="9">
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
-      <c r="F121" s="9">
-        <f>RANK(F117,($C117:$J117))</f>
+      <c r="G121" s="9">
+        <f t="shared" si="23"/>
+        <v>6</v>
+      </c>
+      <c r="H121" s="9">
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="G121" s="9">
-        <f>RANK(G117,($C117:$J117))</f>
-        <v>5</v>
-      </c>
-      <c r="H121" s="9">
-        <f>RANK(H117,($C117:$J117))</f>
+      <c r="I121" s="9">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="J121" s="9">
+        <f t="shared" si="23"/>
+        <v>9</v>
+      </c>
+      <c r="K121" s="9">
+        <f t="shared" si="23"/>
         <v>7</v>
       </c>
-      <c r="I121" s="9">
-        <f>RANK(I117,($C117:$J117))</f>
-        <v>8</v>
-      </c>
-      <c r="J121" s="9">
-        <f>RANK(J117,($C117:$J117))</f>
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M91:P101">
+    <sortCondition ref="P91:P101"/>
+  </sortState>
   <conditionalFormatting sqref="C4:J22">
-    <cfRule type="colorScale" priority="135">
+    <cfRule type="colorScale" priority="141">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5329,7 +5748,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:J22">
-    <cfRule type="colorScale" priority="134">
+    <cfRule type="colorScale" priority="140">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5341,7 +5760,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:J22">
-    <cfRule type="colorScale" priority="125">
+    <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5353,7 +5772,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:J22">
-    <cfRule type="colorScale" priority="114">
+    <cfRule type="colorScale" priority="120">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5365,7 +5784,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:T22">
-    <cfRule type="colorScale" priority="113">
+    <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5377,7 +5796,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:T22 C4:J22">
-    <cfRule type="colorScale" priority="122">
+    <cfRule type="colorScale" priority="128">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5388,8 +5807,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="121">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5400,8 +5819,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="120">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5412,8 +5831,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="119">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5424,8 +5843,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="118">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5436,8 +5855,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="117">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5448,8 +5867,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="109">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5460,8 +5879,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:T54">
-    <cfRule type="colorScale" priority="112">
+  <conditionalFormatting sqref="M24:T25">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5472,8 +5891,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M33:T51">
-    <cfRule type="colorScale" priority="110">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5484,8 +5903,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M33:T51">
-    <cfRule type="colorScale" priority="111">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5496,8 +5915,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="108">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5508,8 +5927,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="107">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5520,8 +5939,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="106">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5532,8 +5951,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="105">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5544,8 +5963,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="104">
+  <conditionalFormatting sqref="C24:J25">
+    <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5556,8 +5975,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="102">
+  <conditionalFormatting sqref="C62:J80">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5568,8 +5987,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:T25">
-    <cfRule type="colorScale" priority="103">
+  <conditionalFormatting sqref="C62:J80">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5580,8 +5999,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="101">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5592,8 +6011,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="100">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5604,8 +6023,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="99">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5616,8 +6035,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="98">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5628,8 +6047,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="97">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5640,8 +6059,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="95">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5652,8 +6071,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J25">
-    <cfRule type="colorScale" priority="96">
+  <conditionalFormatting sqref="C82:J83">
+    <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5664,8 +6083,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62:J80">
-    <cfRule type="colorScale" priority="87">
+  <conditionalFormatting sqref="C62:J80 C82:J83">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5676,8 +6095,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62:J80">
-    <cfRule type="colorScale" priority="88">
+  <conditionalFormatting sqref="C4:J25">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5688,8 +6107,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="85">
+  <conditionalFormatting sqref="M4:T25">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5700,8 +6119,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="84">
+  <conditionalFormatting sqref="C62:J83">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5712,8 +6131,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="83">
+  <conditionalFormatting sqref="C33:J51">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5724,8 +6143,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="82">
+  <conditionalFormatting sqref="C33:J51">
+    <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5736,8 +6155,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="81">
+  <conditionalFormatting sqref="C33:J51">
+    <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5748,8 +6167,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="79">
+  <conditionalFormatting sqref="C33:J51">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5760,8 +6179,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:J83">
-    <cfRule type="colorScale" priority="80">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5772,8 +6191,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62:J80 C82:J83">
-    <cfRule type="colorScale" priority="78">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5784,8 +6203,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M33:T51 M53:T54">
-    <cfRule type="colorScale" priority="77">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5796,8 +6215,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:J25">
-    <cfRule type="colorScale" priority="76">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5808,8 +6227,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:T25">
-    <cfRule type="colorScale" priority="75">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5820,8 +6239,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M33:T54">
-    <cfRule type="colorScale" priority="58">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5832,8 +6251,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62:J83">
-    <cfRule type="colorScale" priority="73">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5844,8 +6263,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:J51">
-    <cfRule type="colorScale" priority="71">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5856,8 +6275,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:J51">
-    <cfRule type="colorScale" priority="72">
+  <conditionalFormatting sqref="C53:J54">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5868,8 +6287,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:J51">
-    <cfRule type="colorScale" priority="70">
+  <conditionalFormatting sqref="C33:J54">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5880,8 +6299,68 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:J51">
-    <cfRule type="colorScale" priority="69">
+  <conditionalFormatting sqref="C85:J86">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:J57">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:J28">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:T28">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N76:U77">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N76:U77">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5892,8 +6371,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="68">
+  <conditionalFormatting sqref="N79:U80">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N91:N101">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5904,8 +6395,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="67">
+  <conditionalFormatting sqref="O91:O101">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5916,8 +6407,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="66">
+  <conditionalFormatting sqref="P91:P101">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5928,8 +6419,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="65">
+  <conditionalFormatting sqref="C91:K113">
+    <cfRule type="colorScale" priority="173">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5940,8 +6431,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="64">
+  <conditionalFormatting sqref="C115:K116">
+    <cfRule type="colorScale" priority="175">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5952,8 +6443,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="62">
+  <conditionalFormatting sqref="C114:K116">
+    <cfRule type="colorScale" priority="177">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5964,8 +6455,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="63">
+  <conditionalFormatting sqref="C119:K121">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91:K116">
+    <cfRule type="colorScale" priority="181">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5976,8 +6479,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="61">
+  <conditionalFormatting sqref="C117:K117">
+    <cfRule type="colorScale" priority="183">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5988,8 +6491,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:J54">
-    <cfRule type="colorScale" priority="60">
+  <conditionalFormatting sqref="C91:K117">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6000,8 +6503,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:J54">
-    <cfRule type="colorScale" priority="57">
+  <conditionalFormatting sqref="M53:T54">
+    <cfRule type="colorScale" priority="184">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6012,8 +6515,44 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85:J86">
-    <cfRule type="colorScale" priority="56">
+  <conditionalFormatting sqref="M33:T51">
+    <cfRule type="colorScale" priority="188">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M33:T51 M53:T54">
+    <cfRule type="colorScale" priority="192">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M33:T54">
+    <cfRule type="colorScale" priority="200">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M56:T57">
+    <cfRule type="colorScale" priority="204">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6024,68 +6563,476 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:J57">
-    <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M56:T57">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27:J28">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M27:T28">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N76:U77">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N76:U77">
-    <cfRule type="colorScale" priority="43">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77953D02-229B-43C1-9222-5F0FDBA4AD43}">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="18">
+        <v>5.7500879999999997E-2</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="18">
+        <v>9.4187530000000005E-2</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.2135206</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.13211545</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.17578205999999999</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0.18440641999999999</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.11383269999999999</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <f>AVERAGE(D3:D10)</f>
+        <v>0.12141820499999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0.10452481</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.18480492600000001</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="18">
+        <v>4.1866342000000001E-2</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="19">
+        <v>4.6130429999999998E-3</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.20704876</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="19">
+        <v>0.15619422199999999</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="19">
+        <v>9.2803775000000005E-2</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0.327868567</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
+        <f>AVERAGE(D14:D21)</f>
+        <v>0.13996555562500002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="19">
+        <v>7.8913300000000006E-2</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="19">
+        <v>0.15011503000000001</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0.26005492000000002</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="18">
+        <v>3.4679269999999998E-2</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="19">
+        <v>0.14835888</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="18">
+        <v>-1.0804940000000001E-2</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="18">
+        <v>0.20680955000000001</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="19">
+        <v>0.15617343</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="19">
+        <v>9.1326190000000002E-2</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="18">
+        <v>0.31010186000000001</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6">
+        <f>AVERAGE(D24:D33)</f>
+        <v>0.142572749</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D24:D33">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6096,20 +7043,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79:U80">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91:J113">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="D14:D21">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6120,295 +7055,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91:J113">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91:J113">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91:J113">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:J116">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C114:J116">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C119:J121">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91:J116">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C117:J117">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91:J117">
+  <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>